<commit_message>
trying to make the code faster
</commit_message>
<xml_diff>
--- a/hw3/Time calculator.xlsx
+++ b/hw3/Time calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chip\source\repos\cs7320_code\hw3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D1CBBF4-967C-4C8A-880A-D00C432C47D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DB36CC-38D3-4CE9-982C-5E4662ECC142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{FCE5153D-B073-4563-B873-7A70D85C5FA3}"/>
+    <workbookView xWindow="11430" yWindow="1515" windowWidth="38700" windowHeight="15435" xr2:uid="{FCE5153D-B073-4563-B873-7A70D85C5FA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,14 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -372,19 +380,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D04ECB-D14D-4F4C-9405-952D5F318F23}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.796875" customWidth="1"/>
-    <col min="3" max="3" width="14.19921875" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>0.46034722222222224</v>
       </c>
@@ -396,7 +404,7 @@
         <v>8.796296296296191E-4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0.49989583333333337</v>
       </c>
@@ -410,6 +418,18 @@
       <c r="E2">
         <f>(29*60)+23</f>
         <v>1763</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>0.59167824074074071</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.57844907407407409</v>
+      </c>
+      <c r="C3" s="1">
+        <f>A3-B3</f>
+        <v>1.3229166666666625E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed main parts of hw3
</commit_message>
<xml_diff>
--- a/hw3/Time calculator.xlsx
+++ b/hw3/Time calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chip\source\repos\cs7320_code\hw3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DB36CC-38D3-4CE9-982C-5E4662ECC142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D527E03-AF1C-49E6-8253-1CC6276A9E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11430" yWindow="1515" windowWidth="38700" windowHeight="15435" xr2:uid="{FCE5153D-B073-4563-B873-7A70D85C5FA3}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{FCE5153D-B073-4563-B873-7A70D85C5FA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,27 +20,63 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+  <si>
+    <t>Board</t>
+  </si>
+  <si>
+    <t># Boards</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>b3</t>
+  </si>
+  <si>
+    <t>31 sec</t>
+  </si>
+  <si>
+    <t>b4</t>
+  </si>
+  <si>
+    <t>892 sec</t>
+  </si>
+  <si>
+    <t>1 sec</t>
+  </si>
+  <si>
+    <t>2 sec</t>
+  </si>
+  <si>
+    <t>MiniMax</t>
+  </si>
+  <si>
+    <t>MiniMaxAB</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -51,7 +87,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -59,13 +95,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -81,6 +145,1156 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Board count: Minimax vs AB Pruning</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>b3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$D$7:$G$8</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Sheet1!$D$7:$D$8,Sheet1!$F$7:$F$8)</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="2"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v># Boards</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v># Boards</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>MiniMax</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>MiniMaxAB</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$D$9:$G$9</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Sheet1!$D$9,Sheet1!$F$9)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="#,##0">
+                  <c:v>549946</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="#,##0">
+                  <c:v>18297</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B2B4-49DD-901A-F4B036B72DDA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>b4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$D$7:$G$8</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Sheet1!$D$7:$D$8,Sheet1!$F$7:$F$8)</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="2"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v># Boards</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v># Boards</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>MiniMax</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>MiniMaxAB</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$D$10:$G$10</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Sheet1!$D$10,Sheet1!$F$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="#,##0">
+                  <c:v>7096505</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="#,##0">
+                  <c:v>29773</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B2B4-49DD-901A-F4B036B72DDA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1278446351"/>
+        <c:axId val="1278445103"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1278446351"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1278445103"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1278445103"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="7500000"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1278446351"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.8457927507194013"/>
+          <c:y val="0.20676456069249605"/>
+          <c:w val="9.6459260278769735E-2"/>
+          <c:h val="5.8742445592781654E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>578787</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>15840</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>174947</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>68034</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A964F4F5-740C-78FD-731C-091E3A272EFB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -380,19 +1594,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D04ECB-D14D-4F4C-9405-952D5F318F23}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.86328125" customWidth="1"/>
+    <col min="3" max="3" width="14.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1">
         <v>0.46034722222222224</v>
       </c>
@@ -404,7 +1618,7 @@
         <v>8.796296296296191E-4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>0.49989583333333337</v>
       </c>
@@ -420,7 +1634,7 @@
         <v>1763</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>0.59167824074074071</v>
       </c>
@@ -432,8 +1646,100 @@
         <v>1.3229166666666625E-2</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" s="1">
+        <v>0.23678240740740741</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.22645833333333332</v>
+      </c>
+      <c r="C4" s="1">
+        <f>A4-B4</f>
+        <v>1.0324074074074097E-2</v>
+      </c>
+      <c r="E4">
+        <f>(60*14) + 52</f>
+        <v>892</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="4">
+        <v>549946</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="4">
+        <v>18297</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="4">
+        <v>7096505</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="4">
+        <v>29773</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C11" s="3"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C12" s="3"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
pushing final homework3 files
</commit_message>
<xml_diff>
--- a/hw3/Time calculator.xlsx
+++ b/hw3/Time calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chip\source\repos\cs7320_code\hw3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FE376B-A266-4EB4-9B2D-06A1A6F5F0E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCA6445-2490-44A7-BCB0-CD986F6F2FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11430" yWindow="1515" windowWidth="38700" windowHeight="15435" xr2:uid="{FCE5153D-B073-4563-B873-7A70D85C5FA3}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{FCE5153D-B073-4563-B873-7A70D85C5FA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Board</t>
   </si>
@@ -50,13 +39,7 @@
     <t>b3</t>
   </si>
   <si>
-    <t>31 sec</t>
-  </si>
-  <si>
     <t>b4</t>
-  </si>
-  <si>
-    <t>892 sec</t>
   </si>
   <si>
     <t>1 sec</t>
@@ -65,10 +48,13 @@
     <t>2 sec</t>
   </si>
   <si>
-    <t>MiniMax</t>
+    <t>MiniMaxAB</t>
   </si>
   <si>
-    <t>MiniMaxAB</t>
+    <t>MiniMaxAB_heuristic</t>
+  </si>
+  <si>
+    <t>5 sec</t>
   </si>
 </sst>
 </file>
@@ -98,7 +84,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -121,11 +107,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -140,6 +137,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -193,7 +196,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Board count: Minimax vs AB Pruning</a:t>
+              <a:t>Board count: MiniMaxAB vs MiniMaxAB_heuristic</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -338,10 +341,10 @@
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>MiniMax</c:v>
+                    <c:v>MiniMaxAB</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>MiniMaxAB</c:v>
+                    <c:v>MiniMaxAB_heuristic</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -361,10 +364,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="#,##0">
-                  <c:v>549946</c:v>
+                  <c:v>18297</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="#,##0">
-                  <c:v>18297</c:v>
+                  <c:v>17423</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -479,10 +482,10 @@
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>MiniMax</c:v>
+                    <c:v>MiniMaxAB</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>MiniMaxAB</c:v>
+                    <c:v>MiniMaxAB_heuristic</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -502,10 +505,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="#,##0">
-                  <c:v>7096505</c:v>
+                  <c:v>29773</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="#,##0">
-                  <c:v>29773</c:v>
+                  <c:v>46781</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -584,7 +587,6 @@
         <c:axId val="1278445103"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="7500000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1271,16 +1273,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>578787</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>15840</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>515611</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>25559</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>174947</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>68034</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>111771</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>77752</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1608,16 +1610,16 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.86328125" customWidth="1"/>
+    <col min="3" max="3" width="14.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1">
         <v>0.46034722222222224</v>
       </c>
@@ -1629,7 +1631,7 @@
         <v>8.796296296296191E-4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>0.49989583333333337</v>
       </c>
@@ -1645,7 +1647,7 @@
         <v>1763</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>0.59167824074074071</v>
       </c>
@@ -1657,7 +1659,7 @@
         <v>1.3229166666666625E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>0.23678240740740741</v>
       </c>
@@ -1673,7 +1675,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>0.28347222222222224</v>
       </c>
@@ -1689,17 +1691,17 @@
         <v>395</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="D7" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C8" s="2" t="s">
         <v>0</v>
       </c>
@@ -1716,46 +1718,44 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="3">
-        <v>549946</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="D9" s="7">
+        <v>18297</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="3">
+        <v>17423</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="3">
-        <v>18297</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>7</v>
+      <c r="D10" s="7">
+        <v>29773</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="3">
+        <v>46781</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="3">
-        <v>7096505</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="3">
-        <v>29773</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>8</v>
-      </c>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C11" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="2"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C12" s="2"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>

</xml_diff>